<commit_message>
Checkpoint and Smart ID demo
</commit_message>
<xml_diff>
--- a/GUITest1/Default.xlsx
+++ b/GUITest1/Default.xlsx
@@ -14,6 +14,20 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>menuCart_innertext</t>
+  </si>
+  <si>
+    <t>menuCart_html_tag</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
@@ -154,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -162,13 +176,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -467,16 +511,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.41796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.67578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row customFormat="1">
+      <c t="s">
+        <v>0</v>
+      </c>
+      <c t="s">
+        <v>2</v>
+      </c>
+      <c t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>2</v>
+      </c>
+      <c s="1"/>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="1">
+        <v>3</v>
+      </c>
+      <c s="1"/>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="1">
+        <v>4</v>
+      </c>
+      <c s="1"/>
+      <c s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -492,7 +572,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>